<commit_message>
minor changes and cleanups
</commit_message>
<xml_diff>
--- a/Inputs_data/NYCTRS_MemberData_AV2016.xlsx
+++ b/Inputs_data/NYCTRS_MemberData_AV2016.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3C4514-0954-4A72-B7C6-778822800CA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E57AFD8-CBBB-4A66-85A1-3DC233B59242}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="770" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" tabRatio="770" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="20" r:id="rId1"/>
@@ -2911,18 +2911,102 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="15"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
     </xf>
@@ -2952,90 +3036,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3955,10 +3955,10 @@
       <c r="E27" s="184">
         <v>14177803</v>
       </c>
-      <c r="F27" s="186" t="s">
+      <c r="F27" s="215" t="s">
         <v>229</v>
       </c>
-      <c r="G27" s="186"/>
+      <c r="G27" s="215"/>
       <c r="H27" s="178">
         <v>42446261</v>
       </c>
@@ -4310,17 +4310,17 @@
       <c r="H48" s="177"/>
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C49" s="186" t="s">
+      <c r="C49" s="215" t="s">
         <v>229</v>
       </c>
-      <c r="D49" s="186"/>
+      <c r="D49" s="215"/>
       <c r="E49" s="130">
         <v>9818763</v>
       </c>
-      <c r="F49" s="186" t="s">
+      <c r="F49" s="215" t="s">
         <v>229</v>
       </c>
-      <c r="G49" s="186"/>
+      <c r="G49" s="215"/>
       <c r="H49" s="178">
         <v>21092711</v>
       </c>
@@ -10221,10 +10221,10 @@
       <c r="E6" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="F6" s="187" t="s">
+      <c r="F6" s="212" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="187"/>
+      <c r="G6" s="212"/>
     </row>
     <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B7" s="98" t="s">
@@ -10543,15 +10543,15 @@
       <c r="G23" s="87"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="188" t="s">
+      <c r="B24" s="217" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="188"/>
-      <c r="D24" s="188"/>
-      <c r="E24" s="189" t="s">
+      <c r="C24" s="217"/>
+      <c r="D24" s="217"/>
+      <c r="E24" s="216" t="s">
         <v>175</v>
       </c>
-      <c r="F24" s="189"/>
+      <c r="F24" s="216"/>
       <c r="G24" s="120">
         <v>42446261</v>
       </c>
@@ -10570,17 +10570,17 @@
       <c r="B30" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="C30" s="187" t="s">
+      <c r="C30" s="212" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="187"/>
+      <c r="D30" s="212"/>
       <c r="E30" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="F30" s="190" t="s">
+      <c r="F30" s="218" t="s">
         <v>178</v>
       </c>
-      <c r="G30" s="190"/>
+      <c r="G30" s="218"/>
     </row>
     <row r="31" spans="2:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B31" s="101" t="s">
@@ -10899,17 +10899,17 @@
       <c r="G47" s="87"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="189" t="s">
+      <c r="B48" s="216" t="s">
         <v>175</v>
       </c>
-      <c r="C48" s="189"/>
+      <c r="C48" s="216"/>
       <c r="D48" s="124">
         <v>9818763</v>
       </c>
-      <c r="E48" s="189" t="s">
+      <c r="E48" s="216" t="s">
         <v>175</v>
       </c>
-      <c r="F48" s="189"/>
+      <c r="F48" s="216"/>
       <c r="G48" s="120">
         <v>21092711</v>
       </c>
@@ -11293,17 +11293,17 @@
       <c r="G22" s="87"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="191" t="s">
+      <c r="B23" s="219" t="s">
         <v>198</v>
       </c>
-      <c r="C23" s="191"/>
+      <c r="C23" s="219"/>
       <c r="D23" s="142">
         <v>34371598</v>
       </c>
-      <c r="E23" s="191" t="s">
+      <c r="E23" s="219" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="191"/>
+      <c r="F23" s="219"/>
       <c r="G23" s="142">
         <v>110963139</v>
       </c>
@@ -11352,26 +11352,26 @@
       <c r="B6" s="143" t="s">
         <v>205</v>
       </c>
-      <c r="C6" s="192" t="s">
+      <c r="C6" s="220" t="s">
         <v>206</v>
       </c>
-      <c r="D6" s="192"/>
-      <c r="E6" s="193" t="s">
+      <c r="D6" s="220"/>
+      <c r="E6" s="221" t="s">
         <v>207</v>
       </c>
-      <c r="F6" s="193"/>
-      <c r="G6" s="192" t="s">
+      <c r="F6" s="221"/>
+      <c r="G6" s="220" t="s">
         <v>208</v>
       </c>
-      <c r="H6" s="192"/>
-      <c r="I6" s="193" t="s">
+      <c r="H6" s="220"/>
+      <c r="I6" s="221" t="s">
         <v>209</v>
       </c>
-      <c r="J6" s="193"/>
-      <c r="K6" s="194" t="s">
+      <c r="J6" s="221"/>
+      <c r="K6" s="222" t="s">
         <v>210</v>
       </c>
-      <c r="L6" s="194"/>
+      <c r="L6" s="222"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="128" t="s">
@@ -11919,31 +11919,31 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="195" t="s">
+      <c r="B5" s="223" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="196" t="s">
+      <c r="C5" s="224" t="s">
         <v>143</v>
       </c>
       <c r="D5" s="87"/>
-      <c r="E5" s="197" t="s">
+      <c r="E5" s="225" t="s">
         <v>144</v>
       </c>
-      <c r="F5" s="197"/>
-      <c r="G5" s="197"/>
-      <c r="H5" s="197"/>
+      <c r="F5" s="225"/>
+      <c r="G5" s="225"/>
+      <c r="H5" s="225"/>
       <c r="I5" s="87"/>
-      <c r="J5" s="198" t="s">
+      <c r="J5" s="226" t="s">
         <v>145</v>
       </c>
-      <c r="K5" s="198"/>
-      <c r="L5" s="198"/>
+      <c r="K5" s="226"/>
+      <c r="L5" s="226"/>
       <c r="M5" s="87"/>
       <c r="N5" s="87"/>
     </row>
     <row r="6" spans="1:14" ht="54" x14ac:dyDescent="0.25">
-      <c r="B6" s="195"/>
-      <c r="C6" s="196"/>
+      <c r="B6" s="223"/>
+      <c r="C6" s="224"/>
       <c r="D6" s="88" t="s">
         <v>146</v>
       </c>
@@ -11971,10 +11971,10 @@
       <c r="L6" s="90" t="s">
         <v>154</v>
       </c>
-      <c r="M6" s="199" t="s">
+      <c r="M6" s="227" t="s">
         <v>155</v>
       </c>
-      <c r="N6" s="199"/>
+      <c r="N6" s="227"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="91">
@@ -12402,7 +12402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF8EEF1-1866-4910-AE47-59453CB830C5}">
   <dimension ref="C3:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -12423,55 +12423,55 @@
       </c>
     </row>
     <row r="6" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="200" t="s">
+      <c r="C6" s="186" t="s">
         <v>205</v>
       </c>
-      <c r="D6" s="201" t="s">
+      <c r="D6" s="211" t="s">
         <v>234</v>
       </c>
-      <c r="E6" s="201"/>
-      <c r="F6" s="202" t="s">
+      <c r="E6" s="211"/>
+      <c r="F6" s="187" t="s">
         <v>205</v>
       </c>
-      <c r="G6" s="187" t="s">
+      <c r="G6" s="212" t="s">
         <v>235</v>
       </c>
-      <c r="H6" s="187"/>
+      <c r="H6" s="212"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="203" t="s">
+      <c r="C7" s="188" t="s">
         <v>236</v>
       </c>
-      <c r="D7" s="204">
+      <c r="D7" s="189">
         <v>486</v>
       </c>
-      <c r="E7" s="205">
+      <c r="E7" s="190">
         <v>49321</v>
       </c>
-      <c r="F7" s="206" t="s">
+      <c r="F7" s="191" t="s">
         <v>236</v>
       </c>
-      <c r="G7" s="207">
+      <c r="G7" s="192">
         <v>1790</v>
       </c>
-      <c r="H7" s="208">
+      <c r="H7" s="193">
         <v>50023</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="209" t="s">
+      <c r="C8" s="194" t="s">
         <v>237</v>
       </c>
-      <c r="D8" s="210">
+      <c r="D8" s="195">
         <v>2769</v>
       </c>
-      <c r="E8" s="211">
+      <c r="E8" s="196">
         <v>60106</v>
       </c>
-      <c r="F8" s="212" t="s">
+      <c r="F8" s="197" t="s">
         <v>237</v>
       </c>
-      <c r="G8" s="213">
+      <c r="G8" s="198">
         <v>10599</v>
       </c>
       <c r="H8" s="72">
@@ -12479,19 +12479,19 @@
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="209" t="s">
+      <c r="C9" s="194" t="s">
         <v>126</v>
       </c>
-      <c r="D9" s="210">
+      <c r="D9" s="195">
         <v>3876</v>
       </c>
-      <c r="E9" s="211">
+      <c r="E9" s="196">
         <v>73936</v>
       </c>
-      <c r="F9" s="212" t="s">
+      <c r="F9" s="197" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="213">
+      <c r="G9" s="198">
         <v>13101</v>
       </c>
       <c r="H9" s="72">
@@ -12499,19 +12499,19 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="209" t="s">
+      <c r="C10" s="194" t="s">
         <v>127</v>
       </c>
-      <c r="D10" s="210">
+      <c r="D10" s="195">
         <v>4007</v>
       </c>
-      <c r="E10" s="211">
+      <c r="E10" s="196">
         <v>83966</v>
       </c>
-      <c r="F10" s="212" t="s">
+      <c r="F10" s="197" t="s">
         <v>127</v>
       </c>
-      <c r="G10" s="213">
+      <c r="G10" s="198">
         <v>12813</v>
       </c>
       <c r="H10" s="72">
@@ -12519,19 +12519,19 @@
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="209" t="s">
+      <c r="C11" s="194" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="210">
+      <c r="D11" s="195">
         <v>3639</v>
       </c>
-      <c r="E11" s="211">
+      <c r="E11" s="196">
         <v>89560</v>
       </c>
-      <c r="F11" s="212" t="s">
+      <c r="F11" s="197" t="s">
         <v>128</v>
       </c>
-      <c r="G11" s="213">
+      <c r="G11" s="198">
         <v>11781</v>
       </c>
       <c r="H11" s="72">
@@ -12539,19 +12539,19 @@
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="209" t="s">
+      <c r="C12" s="194" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="210">
+      <c r="D12" s="195">
         <v>3417</v>
       </c>
-      <c r="E12" s="211">
+      <c r="E12" s="196">
         <v>91446</v>
       </c>
-      <c r="F12" s="212" t="s">
+      <c r="F12" s="197" t="s">
         <v>129</v>
       </c>
-      <c r="G12" s="213">
+      <c r="G12" s="198">
         <v>11430</v>
       </c>
       <c r="H12" s="72">
@@ -12559,19 +12559,19 @@
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="209" t="s">
+      <c r="C13" s="194" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="210">
+      <c r="D13" s="195">
         <v>3021</v>
       </c>
-      <c r="E13" s="211">
+      <c r="E13" s="196">
         <v>93611</v>
       </c>
-      <c r="F13" s="212" t="s">
+      <c r="F13" s="197" t="s">
         <v>130</v>
       </c>
-      <c r="G13" s="213">
+      <c r="G13" s="198">
         <v>10784</v>
       </c>
       <c r="H13" s="72">
@@ -12579,19 +12579,19 @@
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="209" t="s">
+      <c r="C14" s="194" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="210">
+      <c r="D14" s="195">
         <v>2505</v>
       </c>
-      <c r="E14" s="211">
+      <c r="E14" s="196">
         <v>92257</v>
       </c>
-      <c r="F14" s="212" t="s">
+      <c r="F14" s="197" t="s">
         <v>131</v>
       </c>
-      <c r="G14" s="213">
+      <c r="G14" s="198">
         <v>9390</v>
       </c>
       <c r="H14" s="72">
@@ -12599,19 +12599,19 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="209" t="s">
+      <c r="C15" s="194" t="s">
         <v>132</v>
       </c>
-      <c r="D15" s="210">
+      <c r="D15" s="195">
         <v>1753</v>
       </c>
-      <c r="E15" s="211">
+      <c r="E15" s="196">
         <v>90102</v>
       </c>
-      <c r="F15" s="212" t="s">
+      <c r="F15" s="197" t="s">
         <v>132</v>
       </c>
-      <c r="G15" s="213">
+      <c r="G15" s="198">
         <v>6616</v>
       </c>
       <c r="H15" s="72">
@@ -12619,19 +12619,19 @@
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="209" t="s">
+      <c r="C16" s="194" t="s">
         <v>133</v>
       </c>
-      <c r="D16" s="214">
+      <c r="D16" s="199">
         <v>841</v>
       </c>
-      <c r="E16" s="211">
+      <c r="E16" s="196">
         <v>82010</v>
       </c>
-      <c r="F16" s="212" t="s">
+      <c r="F16" s="197" t="s">
         <v>133</v>
       </c>
-      <c r="G16" s="213">
+      <c r="G16" s="198">
         <v>2528</v>
       </c>
       <c r="H16" s="72">
@@ -12639,19 +12639,19 @@
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="215" t="s">
+      <c r="C17" s="200" t="s">
         <v>238</v>
       </c>
-      <c r="D17" s="216">
+      <c r="D17" s="201">
         <v>335</v>
       </c>
-      <c r="E17" s="217">
+      <c r="E17" s="202">
         <v>81596</v>
       </c>
-      <c r="F17" s="218" t="s">
+      <c r="F17" s="203" t="s">
         <v>238</v>
       </c>
-      <c r="G17" s="219">
+      <c r="G17" s="204">
         <v>720</v>
       </c>
       <c r="H17" s="78">
@@ -12659,36 +12659,36 @@
       </c>
     </row>
     <row r="18" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="220" t="s">
+      <c r="C18" s="205" t="s">
         <v>139</v>
       </c>
-      <c r="D18" s="221">
+      <c r="D18" s="206">
         <v>26649</v>
       </c>
-      <c r="E18" s="222">
+      <c r="E18" s="207">
         <v>83304</v>
       </c>
-      <c r="F18" s="223" t="s">
+      <c r="F18" s="208" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="224">
+      <c r="G18" s="209">
         <v>91552</v>
       </c>
-      <c r="H18" s="225">
+      <c r="H18" s="210">
         <v>76506</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="226" t="s">
+      <c r="C19" s="213" t="s">
         <v>239</v>
       </c>
-      <c r="D19" s="226"/>
-      <c r="E19" s="227" t="s">
+      <c r="D19" s="213"/>
+      <c r="E19" s="214" t="s">
         <v>240</v>
       </c>
-      <c r="F19" s="227"/>
-      <c r="G19" s="227"/>
-      <c r="H19" s="208">
+      <c r="F19" s="214"/>
+      <c r="G19" s="214"/>
+      <c r="H19" s="193">
         <v>7004302989</v>
       </c>
     </row>
@@ -12707,8 +12707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13772,7 +13772,7 @@
   <dimension ref="C3:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="F29" sqref="F29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13792,55 +13792,55 @@
       </c>
     </row>
     <row r="6" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="200" t="s">
+      <c r="C6" s="186" t="s">
         <v>205</v>
       </c>
-      <c r="D6" s="201" t="s">
+      <c r="D6" s="211" t="s">
         <v>234</v>
       </c>
-      <c r="E6" s="201"/>
-      <c r="F6" s="202" t="s">
+      <c r="E6" s="211"/>
+      <c r="F6" s="187" t="s">
         <v>205</v>
       </c>
-      <c r="G6" s="187" t="s">
+      <c r="G6" s="212" t="s">
         <v>235</v>
       </c>
-      <c r="H6" s="187"/>
+      <c r="H6" s="212"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="203" t="s">
+      <c r="C7" s="188" t="s">
         <v>236</v>
       </c>
-      <c r="D7" s="204">
+      <c r="D7" s="189">
         <v>486</v>
       </c>
-      <c r="E7" s="205">
+      <c r="E7" s="190">
         <v>49321</v>
       </c>
-      <c r="F7" s="206" t="s">
+      <c r="F7" s="191" t="s">
         <v>236</v>
       </c>
-      <c r="G7" s="207">
+      <c r="G7" s="192">
         <v>1790</v>
       </c>
-      <c r="H7" s="208">
+      <c r="H7" s="193">
         <v>50023</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="209" t="s">
+      <c r="C8" s="194" t="s">
         <v>237</v>
       </c>
-      <c r="D8" s="210">
+      <c r="D8" s="195">
         <v>2769</v>
       </c>
-      <c r="E8" s="211">
+      <c r="E8" s="196">
         <v>60106</v>
       </c>
-      <c r="F8" s="212" t="s">
+      <c r="F8" s="197" t="s">
         <v>237</v>
       </c>
-      <c r="G8" s="213">
+      <c r="G8" s="198">
         <v>10599</v>
       </c>
       <c r="H8" s="72">
@@ -13848,19 +13848,19 @@
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="209" t="s">
+      <c r="C9" s="194" t="s">
         <v>126</v>
       </c>
-      <c r="D9" s="210">
+      <c r="D9" s="195">
         <v>3876</v>
       </c>
-      <c r="E9" s="211">
+      <c r="E9" s="196">
         <v>73936</v>
       </c>
-      <c r="F9" s="212" t="s">
+      <c r="F9" s="197" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="213">
+      <c r="G9" s="198">
         <v>13101</v>
       </c>
       <c r="H9" s="72">
@@ -13868,19 +13868,19 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="209" t="s">
+      <c r="C10" s="194" t="s">
         <v>127</v>
       </c>
-      <c r="D10" s="210">
+      <c r="D10" s="195">
         <v>4007</v>
       </c>
-      <c r="E10" s="211">
+      <c r="E10" s="196">
         <v>83966</v>
       </c>
-      <c r="F10" s="212" t="s">
+      <c r="F10" s="197" t="s">
         <v>127</v>
       </c>
-      <c r="G10" s="213">
+      <c r="G10" s="198">
         <v>12813</v>
       </c>
       <c r="H10" s="72">
@@ -13888,19 +13888,19 @@
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="209" t="s">
+      <c r="C11" s="194" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="210">
+      <c r="D11" s="195">
         <v>3639</v>
       </c>
-      <c r="E11" s="211">
+      <c r="E11" s="196">
         <v>89560</v>
       </c>
-      <c r="F11" s="212" t="s">
+      <c r="F11" s="197" t="s">
         <v>128</v>
       </c>
-      <c r="G11" s="213">
+      <c r="G11" s="198">
         <v>11781</v>
       </c>
       <c r="H11" s="72">
@@ -13908,19 +13908,19 @@
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="209" t="s">
+      <c r="C12" s="194" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="210">
+      <c r="D12" s="195">
         <v>3417</v>
       </c>
-      <c r="E12" s="211">
+      <c r="E12" s="196">
         <v>91446</v>
       </c>
-      <c r="F12" s="212" t="s">
+      <c r="F12" s="197" t="s">
         <v>129</v>
       </c>
-      <c r="G12" s="213">
+      <c r="G12" s="198">
         <v>11430</v>
       </c>
       <c r="H12" s="72">
@@ -13928,19 +13928,19 @@
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="209" t="s">
+      <c r="C13" s="194" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="210">
+      <c r="D13" s="195">
         <v>3021</v>
       </c>
-      <c r="E13" s="211">
+      <c r="E13" s="196">
         <v>93611</v>
       </c>
-      <c r="F13" s="212" t="s">
+      <c r="F13" s="197" t="s">
         <v>130</v>
       </c>
-      <c r="G13" s="213">
+      <c r="G13" s="198">
         <v>10784</v>
       </c>
       <c r="H13" s="72">
@@ -13948,19 +13948,19 @@
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="209" t="s">
+      <c r="C14" s="194" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="210">
+      <c r="D14" s="195">
         <v>2505</v>
       </c>
-      <c r="E14" s="211">
+      <c r="E14" s="196">
         <v>92257</v>
       </c>
-      <c r="F14" s="212" t="s">
+      <c r="F14" s="197" t="s">
         <v>131</v>
       </c>
-      <c r="G14" s="213">
+      <c r="G14" s="198">
         <v>9390</v>
       </c>
       <c r="H14" s="72">
@@ -13968,19 +13968,19 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="209" t="s">
+      <c r="C15" s="194" t="s">
         <v>132</v>
       </c>
-      <c r="D15" s="210">
+      <c r="D15" s="195">
         <v>1753</v>
       </c>
-      <c r="E15" s="211">
+      <c r="E15" s="196">
         <v>90102</v>
       </c>
-      <c r="F15" s="212" t="s">
+      <c r="F15" s="197" t="s">
         <v>132</v>
       </c>
-      <c r="G15" s="213">
+      <c r="G15" s="198">
         <v>6616</v>
       </c>
       <c r="H15" s="72">
@@ -13988,19 +13988,19 @@
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="209" t="s">
+      <c r="C16" s="194" t="s">
         <v>133</v>
       </c>
-      <c r="D16" s="214">
+      <c r="D16" s="199">
         <v>841</v>
       </c>
-      <c r="E16" s="211">
+      <c r="E16" s="196">
         <v>82010</v>
       </c>
-      <c r="F16" s="212" t="s">
+      <c r="F16" s="197" t="s">
         <v>133</v>
       </c>
-      <c r="G16" s="213">
+      <c r="G16" s="198">
         <v>2528</v>
       </c>
       <c r="H16" s="72">
@@ -14008,19 +14008,19 @@
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="215" t="s">
+      <c r="C17" s="200" t="s">
         <v>238</v>
       </c>
-      <c r="D17" s="216">
+      <c r="D17" s="201">
         <v>335</v>
       </c>
-      <c r="E17" s="217">
+      <c r="E17" s="202">
         <v>81596</v>
       </c>
-      <c r="F17" s="218" t="s">
+      <c r="F17" s="203" t="s">
         <v>238</v>
       </c>
-      <c r="G17" s="219">
+      <c r="G17" s="204">
         <v>720</v>
       </c>
       <c r="H17" s="78">
@@ -14028,36 +14028,36 @@
       </c>
     </row>
     <row r="18" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="220" t="s">
+      <c r="C18" s="205" t="s">
         <v>139</v>
       </c>
-      <c r="D18" s="221">
+      <c r="D18" s="206">
         <v>26649</v>
       </c>
-      <c r="E18" s="222">
+      <c r="E18" s="207">
         <v>83304</v>
       </c>
-      <c r="F18" s="223" t="s">
+      <c r="F18" s="208" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="224">
+      <c r="G18" s="209">
         <v>91552</v>
       </c>
-      <c r="H18" s="225">
+      <c r="H18" s="210">
         <v>76506</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="226" t="s">
+      <c r="C19" s="213" t="s">
         <v>239</v>
       </c>
-      <c r="D19" s="226"/>
-      <c r="E19" s="227" t="s">
+      <c r="D19" s="213"/>
+      <c r="E19" s="214" t="s">
         <v>240</v>
       </c>
-      <c r="F19" s="227"/>
-      <c r="G19" s="227"/>
-      <c r="H19" s="208">
+      <c r="F19" s="214"/>
+      <c r="G19" s="214"/>
+      <c r="H19" s="193">
         <v>7004302989</v>
       </c>
     </row>

</xml_diff>